<commit_message>
minimize average time method selected and randomized
</commit_message>
<xml_diff>
--- a/constructive-method/solutions/Data_40_Salidas_composición_zonas_heterogéneas.xlsx_nearest_neighbor_minimize_avg_time.xlsx
+++ b/constructive-method/solutions/Data_40_Salidas_composición_zonas_heterogéneas.xlsx_nearest_neighbor_minimize_avg_time.xlsx
@@ -464,7 +464,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>834.6095523840416</v>
+        <v>641.831360147043</v>
       </c>
     </row>
   </sheetData>
@@ -518,7 +518,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>S005</t>
+          <t>S025</t>
         </is>
       </c>
     </row>
@@ -530,7 +530,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>S002</t>
+          <t>S029</t>
         </is>
       </c>
     </row>
@@ -542,7 +542,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>S006</t>
+          <t>S005</t>
         </is>
       </c>
     </row>
@@ -554,7 +554,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>S003</t>
+          <t>S026</t>
         </is>
       </c>
     </row>
@@ -566,7 +566,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>S007</t>
+          <t>S002</t>
         </is>
       </c>
     </row>
@@ -578,7 +578,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>S004</t>
+          <t>S030</t>
         </is>
       </c>
     </row>
@@ -590,7 +590,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>S008</t>
+          <t>S006</t>
         </is>
       </c>
     </row>
@@ -602,7 +602,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>S009</t>
+          <t>S027</t>
         </is>
       </c>
     </row>
@@ -614,7 +614,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>S013</t>
+          <t>S003</t>
         </is>
       </c>
     </row>
@@ -626,7 +626,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>S010</t>
+          <t>S007</t>
         </is>
       </c>
     </row>
@@ -638,7 +638,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>S014</t>
+          <t>S031</t>
         </is>
       </c>
     </row>
@@ -650,19 +650,19 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>S011</t>
+          <t>S028</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Pedido_14</t>
+          <t>Pedido_40</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>S015</t>
+          <t>S004</t>
         </is>
       </c>
     </row>
@@ -674,19 +674,19 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>S012</t>
+          <t>S008</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Pedido_40</t>
+          <t>Pedido_14</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>S016</t>
+          <t>S032</t>
         </is>
       </c>
     </row>
@@ -698,7 +698,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>S017</t>
+          <t>S033</t>
         </is>
       </c>
     </row>
@@ -710,43 +710,43 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>S021</t>
+          <t>S009</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Pedido_4</t>
+          <t>Pedido_19</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>S018</t>
+          <t>S013</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Pedido_13</t>
+          <t>Pedido_4</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>S022</t>
+          <t>S037</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Pedido_19</t>
+          <t>Pedido_13</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>S019</t>
+          <t>S010</t>
         </is>
       </c>
     </row>
@@ -758,7 +758,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>S023</t>
+          <t>S034</t>
         </is>
       </c>
     </row>
@@ -770,7 +770,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>S020</t>
+          <t>S038</t>
         </is>
       </c>
     </row>
@@ -782,7 +782,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>S024</t>
+          <t>S014</t>
         </is>
       </c>
     </row>
@@ -794,7 +794,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>S025</t>
+          <t>S035</t>
         </is>
       </c>
     </row>
@@ -806,7 +806,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>S029</t>
+          <t>S011</t>
         </is>
       </c>
     </row>
@@ -818,7 +818,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>S026</t>
+          <t>S039</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>S030</t>
+          <t>S015</t>
         </is>
       </c>
     </row>
@@ -842,43 +842,43 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>S027</t>
+          <t>S036</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Pedido_1</t>
+          <t>Pedido_32</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>S031</t>
+          <t>S012</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Pedido_26</t>
+          <t>Pedido_1</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>S028</t>
+          <t>S016</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Pedido_32</t>
+          <t>Pedido_26</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>S032</t>
+          <t>S040</t>
         </is>
       </c>
     </row>
@@ -890,7 +890,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>S033</t>
+          <t>S017</t>
         </is>
       </c>
     </row>
@@ -902,7 +902,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>S037</t>
+          <t>S021</t>
         </is>
       </c>
     </row>
@@ -914,7 +914,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>S034</t>
+          <t>S018</t>
         </is>
       </c>
     </row>
@@ -926,7 +926,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>S038</t>
+          <t>S022</t>
         </is>
       </c>
     </row>
@@ -938,7 +938,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>S035</t>
+          <t>S019</t>
         </is>
       </c>
     </row>
@@ -950,7 +950,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>S039</t>
+          <t>S023</t>
         </is>
       </c>
     </row>
@@ -962,7 +962,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>S036</t>
+          <t>S020</t>
         </is>
       </c>
     </row>
@@ -974,7 +974,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>S040</t>
+          <t>S024</t>
         </is>
       </c>
     </row>
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>834.6095523840416</v>
+        <v>641.831360147043</v>
       </c>
     </row>
     <row r="3">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>289.3931776408261</v>
+        <v>450.790896313115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>